<commit_message>
Added missing files for Jharkhand
</commit_message>
<xml_diff>
--- a/rto_wise_data/2022/Jharkhand(25)/HAZARIBAG - JH2( 19-JAN-2017 ).xlsx
+++ b/rto_wise_data/2022/Jharkhand(25)/HAZARIBAG - JH2( 19-JAN-2017 ).xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="36">
   <si>
     <t>Maker Month Wise Data  of HAZARIBAG - JH2 , Jharkhand (2022)</t>
   </si>
@@ -66,6 +66,60 @@
   </si>
   <si>
     <t>DEC</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>AMPERE VEHICLES PRIVATE LIMITED</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>BATTRE ELECTRIC MOBLITY PVT LTD</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>HERO ELECTRIC VEHICLES PVT. LTD</t>
+  </si>
+  <si>
+    <t>OLA ELECTRIC TECHNOLOGIES PVT LTD</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>TVS MOTOR COMPANY LTD</t>
+  </si>
+  <si>
+    <t>WUXI SAIGE ELECTRIC (IMPORTER: DELTA AUTOCORP LLP)</t>
   </si>
 </sst>
 </file>
@@ -116,28 +170,38 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="1.04296875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="1.04296875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="2.2109375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="54.78125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="4.2109375" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="4.515625" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="5.15234375" customWidth="true" bestFit="true"/>
@@ -150,7 +214,7 @@
     <col min="12" max="12" width="4.88671875" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="5.11328125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="4.89453125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="1.04296875" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="3.37890625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -222,7 +286,289 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9"/>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" t="s">
+        <v>24</v>
+      </c>
+      <c r="N6" t="s">
+        <v>26</v>
+      </c>
+      <c r="O6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" t="s">
+        <v>18</v>
+      </c>
+      <c r="L7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M7" t="s">
+        <v>20</v>
+      </c>
+      <c r="N7" t="s">
+        <v>20</v>
+      </c>
+      <c r="O7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M8" t="s">
+        <v>32</v>
+      </c>
+      <c r="N8" t="s">
+        <v>26</v>
+      </c>
+      <c r="O8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" t="s">
+        <v>20</v>
+      </c>
+      <c r="K9" t="s">
+        <v>20</v>
+      </c>
+      <c r="L9" t="s">
+        <v>20</v>
+      </c>
+      <c r="M9" t="s">
+        <v>20</v>
+      </c>
+      <c r="N9" t="s">
+        <v>18</v>
+      </c>
+      <c r="O9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" t="s">
+        <v>20</v>
+      </c>
+      <c r="K10" t="s">
+        <v>24</v>
+      </c>
+      <c r="L10" t="s">
+        <v>20</v>
+      </c>
+      <c r="M10" t="s">
+        <v>18</v>
+      </c>
+      <c r="N10" t="s">
+        <v>20</v>
+      </c>
+      <c r="O10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:O1"/>

</xml_diff>